<commit_message>
bổ sung export cho monitor sale man
</commit_message>
<xml_diff>
--- a/DMS/Templates/Monitor_Store_Checker_Report.xlsx
+++ b/DMS/Templates/Monitor_Store_Checker_Report.xlsx
@@ -241,6 +241,12 @@
     </xf>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -249,12 +255,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -536,13 +536,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" style="2" customWidth="1"/>
     <col min="2" max="2" width="9.140625" style="2" bestFit="1" customWidth="1"/>
@@ -614,27 +617,27 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="11"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="13"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="10" t="s">
         <v>25</v>
       </c>
       <c r="D9" s="6" t="s">

</xml_diff>